<commit_message>
Se añaden los entregables de Andreina y Ángel revisados y corregidos por Luis y Devon
</commit_message>
<xml_diff>
--- a/Entregables corregidos Andreina-Ángel/MatrizDeRiesgos.xlsx
+++ b/Entregables corregidos Andreina-Ángel/MatrizDeRiesgos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\Sofka U\Recursos utilizados\Entregables Andreina-Angel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\Sofka U\2024-C1-QA-FP-T02\Entregables corregidos Andreina-Ángel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BD330D-9310-40E9-814D-4071446D8145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3A82AC-A00E-49D9-8698-74CF82C2C53B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -275,9 +275,6 @@
     <t>Realizar pruebas exhaustivas y capacitacion del equipo</t>
   </si>
   <si>
-    <t>CBA: 4-Mala Comunicación</t>
-  </si>
-  <si>
     <t>Implementar acciones para mejorar la comunicación en el equipo</t>
   </si>
   <si>
@@ -344,13 +341,16 @@
     <t>Dificultades financieras, retrasos en la finalización del proyecto o necesidad de reducir funcionalidades o recursos por desviaciones del presupuesto.</t>
   </si>
   <si>
-    <t>Retrasos en la entrega, baja calidad debido a falta de experiencia del equipo.</t>
-  </si>
-  <si>
-    <t>Retrasos en el proyecto debiado a una comunicación deficiente en el equipo</t>
-  </si>
-  <si>
     <t>Afectación de la calidad del producto debido a conflictos internos en el equipo</t>
+  </si>
+  <si>
+    <t>Retrasos en la entrega, baja calidad debido a falta de experiencia del equipo en metodologías ágiles.</t>
+  </si>
+  <si>
+    <t>CBA: 4- Dificultad en la Comunicación</t>
+  </si>
+  <si>
+    <t>Retrasos en el proyecto debido a una comunicación deficiente en el equipo</t>
   </si>
 </sst>
 </file>
@@ -1023,8 +1023,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AV303"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1099,7 +1099,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>10</v>
@@ -1137,7 +1137,7 @@
         <v>45362</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>40</v>
@@ -1212,7 +1212,7 @@
         <v>45363</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>41</v>
@@ -1253,7 +1253,7 @@
         <v>45364</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>42</v>
@@ -1294,7 +1294,7 @@
         <v>45365</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>43</v>
@@ -1335,7 +1335,7 @@
         <v>45366</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>44</v>
@@ -1376,7 +1376,7 @@
         <v>45367</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>58</v>
@@ -1417,7 +1417,7 @@
         <v>45368</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>61</v>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="N9" s="6"/>
     </row>
-    <row r="10" spans="1:48" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>54</v>
       </c>
@@ -1499,13 +1499,13 @@
         <v>45370</v>
       </c>
       <c r="D11" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="F11" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="G11" s="15" t="s">
         <v>63</v>
@@ -1540,13 +1540,13 @@
         <v>45371</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E12" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>76</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>77</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>63</v>
@@ -5496,7 +5496,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
@@ -5504,7 +5504,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
@@ -5512,7 +5512,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
@@ -5520,7 +5520,7 @@
         <v>14</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5548,7 +5548,7 @@
         <v>21</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
@@ -5556,7 +5556,7 @@
         <v>22</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
@@ -5564,7 +5564,7 @@
         <v>23</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5572,7 +5572,7 @@
         <v>24</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5593,17 +5593,17 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -5613,23 +5613,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101000B674BCD04104143B925E94D13EE63D6" ma:contentTypeVersion="8" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="02a8e9dbe448fde3d28822232c77ecba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="99c78fe733576f46bbe313b297c8672b" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3/fields"/>
@@ -5755,31 +5738,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51D06A13-7C9B-4B18-BB8A-77CA0E1B2E6E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA2A1C89-8A51-4743-A56F-F8C5CF25D0ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9024F26D-946A-4EA8-A6DE-31008C1E0148}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5795,4 +5771,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA2A1C89-8A51-4743-A56F-F8C5CF25D0ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51D06A13-7C9B-4B18-BB8A-77CA0E1B2E6E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>